<commit_message>
Aggiunto loop per mandare messaggi singolarmente + log per singolo messaggio inviato
</commit_message>
<xml_diff>
--- a/addressbook/addresses.xlsx
+++ b/addressbook/addresses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\localSites\NodeMailer\addressbook\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\localSites\Jmailer\addressbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F26C7E1-5D52-4674-BA96-046EA8391503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36A751B-443C-4CF1-9413-198942CE8864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="1335" windowWidth="21600" windowHeight="11505" xr2:uid="{B064F148-654C-4C08-8253-C73EBAFF2FA9}"/>
+    <workbookView xWindow="4365" yWindow="3975" windowWidth="21600" windowHeight="11505" xr2:uid="{B064F148-654C-4C08-8253-C73EBAFF2FA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,20 +30,20 @@
     <t>ADDRESSES</t>
   </si>
   <si>
-    <t>aaa@sample.xyz</t>
+    <t>gianluca.marchitelli14@gmail.com</t>
   </si>
   <si>
-    <t>bbb@sample.xyz</t>
+    <t>hello@johnnybrr.site</t>
   </si>
   <si>
-    <t>ccc@sample.xyz</t>
+    <t>gianluca_marchitelli@yahoo.it</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,6 +55,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -83,16 +91,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -405,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6D5E55-2AD3-4FB2-9C3A-CFB2CE9BC6C7}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A252"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A4" sqref="A3:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,26 +433,30 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252" s="2"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{A65D8035-1330-4477-9DA0-FB421F774F9E}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{A37DDA36-8E27-4A3F-B926-B0FBAFDB396A}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{8BC3C5B0-C871-488F-914A-A432BB38801C}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{63C2F00A-D7DA-442C-A54D-BF5D0B071201}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{A682B407-0A9A-413B-9A3C-21DDF0AE45E8}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{60037C07-2308-40FA-A9AA-6F9A45C9787E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>